<commit_message>
comment translation, update retreived information from config file and add some fields
</commit_message>
<xml_diff>
--- a/auxiliar/config.xlsx
+++ b/auxiliar/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\maeee\auxiliar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\projetos\mae\maeee\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F59014-2FE2-4826-88D0-177507FF845A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F778FC-6687-484C-B046-A53B035CBF72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D732A6FF-66EF-4E21-8577-BA7FE68905D0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D732A6FF-66EF-4E21-8577-BA7FE68905D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Empresa:</t>
   </si>
@@ -92,7 +92,37 @@
     <t>Ter header:</t>
   </si>
   <si>
-    <t>false</t>
+    <t>Número máximo de ingredientes:</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Nome ficha:</t>
+  </si>
+  <si>
+    <t>Feuil1</t>
+  </si>
+  <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Preparation number</t>
+  </si>
+  <si>
+    <t>UFI code notified</t>
+  </si>
+  <si>
+    <t>UFI code calculated</t>
+  </si>
+  <si>
+    <t>EuPCS</t>
   </si>
 </sst>
 </file>
@@ -151,13 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -172,6 +199,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,106 +521,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FE307A-BE67-41E0-AA21-B59C004D3E28}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>